<commit_message>
Updated README and .xlsx
</commit_message>
<xml_diff>
--- a/Assignment 1/RTP_Assign1_deliverableL.xlsx
+++ b/Assignment 1/RTP_Assign1_deliverableL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Documents\Semester6_\Real-Time Programming\Assignments\Assignment 1\cst8244_assign1_kund0003_czer0005\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITrepositories\CST8244-Real-Time-Programming\Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8892B1D2-75AD-4666-B081-C790C5204ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15979F04-9E02-4178-AF2A-C680D28EA93D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{53CC6DC9-109D-4130-AD3D-DE80029FC6AF}"/>
   </bookViews>
@@ -288,12 +288,6 @@
     <t xml:space="preserve">Assignment 1 </t>
   </si>
   <si>
-    <t>Josef Kundinger-Markhauser 040824003</t>
-  </si>
-  <si>
-    <t>Patrick Czermak 040389514</t>
-  </si>
-  <si>
     <t xml:space="preserve">E. STATE DIAGRAM (Diagram showing the state machine - SEE ADDITIONAL ATTACHEMENT: </t>
   </si>
   <si>
@@ -310,6 +304,12 @@
   </si>
   <si>
     <t>* EACH STATE CAN SUCCESSFULLY TRANSITION TO EXIT ON input "exit"</t>
+  </si>
+  <si>
+    <t>Josef Kundinger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patrick Czermak </t>
   </si>
 </sst>
 </file>
@@ -530,6 +530,186 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>150812</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>365125</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1E8AF5A-FC63-FAB6-4F60-AD3CD939FCB3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="14033500"/>
+          <a:ext cx="2182813" cy="230188"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>293688</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>7938</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>492125</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectangle 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB0E64BE-85E7-313B-5C84-D6859A287466}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="293688" y="19137313"/>
+          <a:ext cx="2166937" cy="246062"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>103188</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>71438</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D556785A-688A-10B2-DA95-A1A16F198916}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1119188" y="23709313"/>
+          <a:ext cx="2174875" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -834,8 +1014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5643FF73-3D65-4CCA-97AE-4A4C85A0232A}">
   <dimension ref="A2:V118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="Q93" sqref="Q93"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -853,7 +1033,7 @@
     </row>
     <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -861,7 +1041,7 @@
     </row>
     <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1038,7 +1218,7 @@
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C35" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
@@ -1123,58 +1303,58 @@
         <v>0</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L37" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="N37" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="O37" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="P37" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Q37" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="R37" s="6" t="s">
         <v>0</v>
       </c>
       <c r="S37" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="T37" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="U37" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="V37" s="1" t="s">
         <v>23</v>
@@ -1189,58 +1369,58 @@
         <v>1</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>1</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K38" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L38" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M38" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="N38" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="O38" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="P38" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Q38" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="R38" s="6" t="s">
         <v>1</v>
       </c>
       <c r="S38" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="T38" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="U38" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="V38" s="1" t="s">
         <v>23</v>
@@ -1249,64 +1429,64 @@
     <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39" s="7"/>
       <c r="B39" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L39" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M39" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="N39" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="O39" s="6" t="s">
         <v>20</v>
       </c>
       <c r="P39" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Q39" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="R39" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="S39" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="T39" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="U39" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="V39" s="1" t="s">
         <v>23</v>
@@ -1318,61 +1498,61 @@
         <v>2</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L40" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M40" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="N40" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="O40" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="P40" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Q40" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="R40" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="S40" s="6" t="s">
         <v>15</v>
       </c>
       <c r="T40" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="U40" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="V40" s="1" t="s">
         <v>23</v>
@@ -1384,61 +1564,61 @@
         <v>3</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L41" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M41" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="N41" s="6" t="s">
         <v>3</v>
       </c>
       <c r="O41" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="P41" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Q41" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="R41" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="S41" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="T41" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="U41" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="V41" s="1" t="s">
         <v>23</v>
@@ -1450,61 +1630,61 @@
         <v>4</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L42" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M42" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="N42" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="O42" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="P42" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Q42" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="R42" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="S42" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="T42" s="6" t="s">
         <v>16</v>
       </c>
       <c r="U42" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="V42" s="1" t="s">
         <v>23</v>
@@ -1516,61 +1696,61 @@
         <v>5</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>13</v>
       </c>
       <c r="L43" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M43" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="N43" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="O43" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="P43" s="6" t="s">
         <v>5</v>
       </c>
       <c r="Q43" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="R43" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="S43" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="T43" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="U43" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="V43" s="1" t="s">
         <v>23</v>
@@ -1582,61 +1762,61 @@
         <v>6</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L44" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M44" s="6" t="s">
         <v>6</v>
       </c>
       <c r="N44" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="O44" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="P44" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Q44" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="R44" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="S44" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="T44" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="U44" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="V44" s="1" t="s">
         <v>23</v>
@@ -1648,61 +1828,61 @@
         <v>7</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L45" s="6" t="s">
         <v>7</v>
       </c>
       <c r="M45" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="N45" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="O45" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="P45" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Q45" s="6" t="s">
         <v>7</v>
       </c>
       <c r="R45" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="S45" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="T45" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="U45" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="V45" s="1" t="s">
         <v>23</v>
@@ -1714,58 +1894,58 @@
         <v>8</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>8</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L46" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M46" s="5" t="s">
         <v>18</v>
       </c>
       <c r="N46" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="O46" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="P46" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Q46" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="R46" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="S46" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="T46" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="U46" s="6" t="s">
         <v>8</v>
@@ -1780,61 +1960,61 @@
         <v>9</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M47" s="5" t="s">
         <v>18</v>
       </c>
       <c r="N47" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="O47" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="P47" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Q47" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="R47" s="6" t="s">
         <v>14</v>
       </c>
       <c r="S47" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="T47" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="U47" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="V47" s="1" t="s">
         <v>23</v>
@@ -2076,20 +2256,20 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C72" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="118" spans="17:17" x14ac:dyDescent="0.3">
       <c r="Q118" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>